<commit_message>
updated indices of algorithms to run for mode 1
</commit_message>
<xml_diff>
--- a/algorithms_results/MultiProcessing_subgroups_results_delta_15000_0.xlsx
+++ b/algorithms_results/MultiProcessing_subgroups_results_delta_15000_0.xlsx
@@ -550,7 +550,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': np.int64(2), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'UndergradMajor': np.int64(2)}</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -566,7 +566,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>{'DevType': np.int64(2), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'DevType': np.int64(2)}</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -582,7 +582,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -598,7 +598,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'SexualOrientation': np.int64(1)}</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -646,7 +646,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'UndergradMajor': np.int64(2)}</t>
+          <t>{'UndergradMajor': np.int64(2), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -678,7 +678,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>{'UndergradMajor': np.int64(2), 'HDI': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'UndergradMajor': np.int64(2)}</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -694,7 +694,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'DevType': np.int64(2)}</t>
+          <t>{'DevType': np.int64(2), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -934,7 +934,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>{'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -998,7 +998,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>{'Hobby': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'Dependents': np.int64(2), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1030,7 +1030,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'Dependents': np.int64(2), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1046,7 +1046,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'HDI': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1062,7 +1062,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'Dependents': np.int64(2), 'SexualOrientation': np.int64(1)}</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1078,7 +1078,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'HDI': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'SexualOrientation': np.int64(1)}</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1094,7 +1094,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>{'HDI': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'Dependents': np.int64(2), 'HDI': np.int64(1)}</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1110,7 +1110,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Gender': np.int64(1), 'Student': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1126,7 +1126,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1142,7 +1142,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>{'HDI': np.int64(1), 'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'Student': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1158,7 +1158,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'Hobby': np.int64(1)}</t>
+          <t>{'Gender': np.int64(1), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1174,7 +1174,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'Hobby': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'Dependents': np.int64(2), 'Gender': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1190,7 +1190,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'HDI': np.int64(1), 'Hobby': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'Gender': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1206,7 +1206,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Hobby': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'Dependents': np.int64(2), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1222,7 +1222,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'HDI': np.int64(1), 'Hobby': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1238,7 +1238,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'SexualOrientation': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1254,257 +1254,257 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'Dependents': np.int64(2), 'Student': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>15339</v>
+        <v>15779</v>
       </c>
       <c r="C47" t="n">
-        <v>12445.08873558062</v>
+        <v>5234.178807957504</v>
       </c>
       <c r="D47" t="n">
-        <v>-518.1607653415285</v>
+        <v>-7729.070692964642</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'HDI': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Dependents': np.int64(2), 'Student': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>20079</v>
+        <v>15339</v>
       </c>
       <c r="C48" t="n">
-        <v>8320.806949419126</v>
+        <v>12445.08873558062</v>
       </c>
       <c r="D48" t="n">
-        <v>-4642.44255150302</v>
+        <v>-518.1607653415285</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Dependents': np.int64(2), 'Student': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'Student': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>15301</v>
+        <v>20079</v>
       </c>
       <c r="C49" t="n">
-        <v>12493.22924053899</v>
+        <v>8320.806949419126</v>
       </c>
       <c r="D49" t="n">
-        <v>-470.0202603831513</v>
+        <v>-4642.44255150302</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'HDI': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'Dependents': np.int64(2), 'SexualOrientation': np.int64(1)}</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>20128</v>
+        <v>15301</v>
       </c>
       <c r="C50" t="n">
-        <v>8058.492947675052</v>
+        <v>12493.22924053899</v>
       </c>
       <c r="D50" t="n">
-        <v>-4904.756553247094</v>
+        <v>-470.0202603831513</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'UndergradMajor': np.int64(2)}</t>
+          <t>{'Student': np.int64(1), 'HDI': np.int64(1), 'SexualOrientation': np.int64(1)}</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>16152</v>
+        <v>20128</v>
       </c>
       <c r="C51" t="n">
-        <v>19730.73379293201</v>
+        <v>8058.492947675052</v>
       </c>
       <c r="D51" t="n">
-        <v>6767.48429200986</v>
+        <v>-4904.756553247094</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'DevType': np.int64(2)}</t>
+          <t>{'SexualOrientation': np.int64(1), 'UndergradMajor': np.int64(2), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>15929</v>
+        <v>16152</v>
       </c>
       <c r="C52" t="n">
-        <v>10271.32109283204</v>
+        <v>19730.73379293201</v>
       </c>
       <c r="D52" t="n">
-        <v>-2691.928408090102</v>
+        <v>6767.48429200986</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'SexualOrientation': np.int64(1), 'DevType': np.int64(2), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>17563</v>
+        <v>15929</v>
       </c>
       <c r="C53" t="n">
-        <v>12896.98458729801</v>
+        <v>10271.32109283204</v>
       </c>
       <c r="D53" t="n">
-        <v>-66.26491362413253</v>
+        <v>-2691.928408090102</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'HDI': np.int64(1)}</t>
+          <t>{'Dependents': np.int64(2), 'SexualOrientation': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>21900</v>
+        <v>17563</v>
       </c>
       <c r="C54" t="n">
-        <v>8524.583644570461</v>
+        <v>12896.98458729801</v>
       </c>
       <c r="D54" t="n">
-        <v>-4438.665856351685</v>
+        <v>-66.26491362413253</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'HDI': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'HDI': np.int64(1), 'SexualOrientation': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>15786</v>
+        <v>21900</v>
       </c>
       <c r="C55" t="n">
-        <v>12632.85656038428</v>
+        <v>8524.583644570461</v>
       </c>
       <c r="D55" t="n">
-        <v>-330.392940537864</v>
+        <v>-4438.665856351685</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'HDI': np.int64(1), 'Dependents': np.int64(2)}</t>
+          <t>{'Dependents': np.int64(2), 'HDI': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>15673</v>
+        <v>15786</v>
       </c>
       <c r="C56" t="n">
-        <v>12988.61598577243</v>
+        <v>12632.85656038428</v>
       </c>
       <c r="D56" t="n">
-        <v>25.36648485028491</v>
+        <v>-330.392940537864</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Dependents': np.int64(2), 'HDI': np.int64(1), 'SexualOrientation': np.int64(1)}</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>18136</v>
+        <v>15673</v>
       </c>
       <c r="C57" t="n">
-        <v>7283.726461989329</v>
+        <v>12988.61598577243</v>
       </c>
       <c r="D57" t="n">
-        <v>-5679.523038932816</v>
+        <v>25.36648485028491</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>{'Gender': np.int64(1), 'HDI': np.int64(1), 'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'Gender': np.int64(1), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>16648</v>
+        <v>18136</v>
       </c>
       <c r="C58" t="n">
-        <v>6709.311194402443</v>
+        <v>7283.726461989329</v>
       </c>
       <c r="D58" t="n">
-        <v>-6253.938306519703</v>
+        <v>-5679.523038932816</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'HDI': np.int64(1), 'Hobby': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'Gender': np.int64(1), 'Student': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>16486</v>
+        <v>16648</v>
       </c>
       <c r="C59" t="n">
-        <v>5663.715061677382</v>
+        <v>6709.311194402443</v>
       </c>
       <c r="D59" t="n">
-        <v>-7299.534439244764</v>
+        <v>-6253.938306519703</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'HDI': np.int64(1), 'Hobby': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'HDI': np.int64(1), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>18306</v>
+        <v>16486</v>
       </c>
       <c r="C60" t="n">
-        <v>6562.835401713361</v>
+        <v>5663.715061677382</v>
       </c>
       <c r="D60" t="n">
-        <v>-6400.414099208785</v>
+        <v>-7299.534439244764</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>{'SexualOrientation': np.int64(1), 'Gender': np.int64(1), 'HDI': np.int64(1), 'Student': np.int64(1)}</t>
+          <t>{'HDI': np.int64(1), 'Gender': np.int64(1), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>19043</v>
+        <v>18306</v>
       </c>
       <c r="C61" t="n">
-        <v>7319.305231565133</v>
+        <v>6562.835401713361</v>
       </c>
       <c r="D61" t="n">
-        <v>-5643.944269357013</v>
+        <v>-6400.414099208785</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>{'HDI': np.int64(1), 'Gender': np.int64(1), 'Student': np.int64(1), 'SexualOrientation': np.int64(1), 'Hobby': np.int64(1)}</t>
+          <t>{'Student': np.int64(1), 'HDI': np.int64(1), 'SexualOrientation': np.int64(1), 'Gender': np.int64(1)}</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>15779</v>
+        <v>19043</v>
       </c>
       <c r="C62" t="n">
-        <v>5234.178807957504</v>
+        <v>7319.305231565133</v>
       </c>
       <c r="D62" t="n">
-        <v>-7729.070692964642</v>
+        <v>-5643.944269357013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>